<commit_message>
Metodo Get para las empresas
</commit_message>
<xml_diff>
--- a/registro_empresas.xlsx
+++ b/registro_empresas.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1814,16 +1814,1095 @@
         <v>3223236339</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D84" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E84" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Nombre del Representante</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Apellido del Representante</v>
+      </c>
+      <c r="D85" t="str">
+        <v>empresa@example.com</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>2312319</v>
+      </c>
+      <c r="B86" t="str">
+        <v>1uan</v>
+      </c>
+      <c r="C86" t="str">
+        <v>2ablo Bautista</v>
+      </c>
+      <c r="D86" t="str">
+        <v>jbauti1123124lavijo@gmail.com</v>
+      </c>
+      <c r="E86" t="str">
+        <v>3223232339</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>23123124</v>
+      </c>
+      <c r="B87" t="str">
+        <v>1ua4vv</v>
+      </c>
+      <c r="C87" t="str">
+        <v>2abo Bautistav</v>
+      </c>
+      <c r="D87" t="str">
+        <v>jbautivv3ijo@gmail.com</v>
+      </c>
+      <c r="E87" t="str">
+        <v>32232362</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D88" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E88" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D89" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E89" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D90" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E90" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D91" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E91" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D92" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E92" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D93" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E93" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D94" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E94" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D95" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E95" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D96" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E96" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D97" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E97" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D98" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E98" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D99" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E99" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B100" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D100" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E100" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D101" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E101" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D102" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E102" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D103" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E103" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D104" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E104" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B105" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C105" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D105" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E105" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B106" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D106" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E106" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B107" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C107" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D107" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E107" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B108" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D108" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E108" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B109" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D109" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E109" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B110" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D110" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E110" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B111" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D111" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E111" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B112" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C112" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D112" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E112" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B113" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C113" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D113" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E113" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B114" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C114" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D114" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E114" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B115" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C115" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D115" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E115" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B116" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C116" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D116" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E116" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>2312312</v>
+      </c>
+      <c r="B117" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C117" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D117" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E117" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="B118" t="str">
+        <v>Nombre del Representante</v>
+      </c>
+      <c r="C118" t="str">
+        <v>Apellido del Representante</v>
+      </c>
+      <c r="D118" t="str">
+        <v>empresa@example.com</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>312311</v>
+      </c>
+      <c r="B119" t="str">
+        <v>Jua21</v>
+      </c>
+      <c r="C119" t="str">
+        <v>Pablo Bautist1a</v>
+      </c>
+      <c r="D119" t="str">
+        <v>jpbautistac@udistrital.edu.co</v>
+      </c>
+      <c r="E119" t="str">
+        <v>3223236331</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>31231108</v>
+      </c>
+      <c r="B120" t="str">
+        <v>Ju</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Pablo Bautis</v>
+      </c>
+      <c r="D120" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E120" t="str">
+        <v>32232363</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>100192812</v>
+      </c>
+      <c r="B121" t="str">
+        <v>Pandebono</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Aguacate</v>
+      </c>
+      <c r="D121" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E121" t="str">
+        <v>4123212</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B122" t="str">
+        <v>Pandebono</v>
+      </c>
+      <c r="C122" t="str">
+        <v>Aguacate</v>
+      </c>
+      <c r="D122" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E122" t="str">
+        <v>3213122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B123" t="str">
+        <v>Pandebono</v>
+      </c>
+      <c r="C123" t="str">
+        <v>Aguacate</v>
+      </c>
+      <c r="D123" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E123" t="str">
+        <v>3213122</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>10045678</v>
+      </c>
+      <c r="B124" t="str">
+        <v>Nombre del Re0entante</v>
+      </c>
+      <c r="C124" t="str">
+        <v>Apellido00 Representante</v>
+      </c>
+      <c r="D124" t="str">
+        <v>empresa@examp12.com</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B125" t="str">
+        <v>Pandebono</v>
+      </c>
+      <c r="C125" t="str">
+        <v>Aguacate</v>
+      </c>
+      <c r="D125" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E125" t="str">
+        <v>3213122</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>32312777</v>
+      </c>
+      <c r="B126" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C126" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D126" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E126" t="str">
+        <v>3213122</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>4122222</v>
+      </c>
+      <c r="B127" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C127" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D127" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E127" t="str">
+        <v>3213122</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>32312777</v>
+      </c>
+      <c r="B128" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C128" t="str">
+        <v>21gdsfgs</v>
+      </c>
+      <c r="D128" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E128" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B129" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C129" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D129" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E129" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B130" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C130" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D130" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E130" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B131" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C131" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D131" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E131" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B132" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C132" t="str">
+        <v>21gdsfgs</v>
+      </c>
+      <c r="D132" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E132" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B133" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C133" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D133" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E133" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B134" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C134" t="str">
+        <v>21gdsfgs</v>
+      </c>
+      <c r="D134" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E134" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B135" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C135" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D135" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E135" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B136" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C136" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D136" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E136" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B137" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C137" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D137" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E137" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B138" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C138" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D138" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E138" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B139" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C139" t="str">
+        <v>21gdsfgs</v>
+      </c>
+      <c r="D139" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E139" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B140" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C140" t="str">
+        <v>21gdsfgs</v>
+      </c>
+      <c r="D140" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E140" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B141" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C141" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D141" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E141" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B142" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C142" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D142" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E142" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B143" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C143" t="str">
+        <v>lelqweqwe</v>
+      </c>
+      <c r="D143" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E143" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>32143123</v>
+      </c>
+      <c r="B144" t="str">
+        <v>kkqw</v>
+      </c>
+      <c r="C144" t="str">
+        <v>21gdsfgs</v>
+      </c>
+      <c r="D144" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E144" t="str">
+        <v>31231288</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>31231108</v>
+      </c>
+      <c r="B145" t="str">
+        <v>Ju</v>
+      </c>
+      <c r="C145" t="str">
+        <v>Pablo Bautis</v>
+      </c>
+      <c r="D145" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E145" t="str">
+        <v>32232363</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>31231108</v>
+      </c>
+      <c r="B146" t="str">
+        <v>Ju</v>
+      </c>
+      <c r="C146" t="str">
+        <v>Pablo Bautis</v>
+      </c>
+      <c r="D146" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E146" t="str">
+        <v>32232363</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>31231108</v>
+      </c>
+      <c r="B147" t="str">
+        <v>Ju</v>
+      </c>
+      <c r="C147" t="str">
+        <v>Pablo Bautis</v>
+      </c>
+      <c r="D147" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E147" t="str">
+        <v>32232363</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E83"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E147"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3488,9 +4567,1280 @@
         <v>2312312</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B84" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C84" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D84" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E84" t="str">
+        <v>9</v>
+      </c>
+      <c r="F84" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Nombre de la Empresa</v>
+      </c>
+      <c r="B85" t="str">
+        <v>33456789</v>
+      </c>
+      <c r="D85" t="str">
+        <v>empresa@example.com</v>
+      </c>
+      <c r="E85" t="str">
+        <v>1</v>
+      </c>
+      <c r="F85" t="str">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>COCA-COLA1</v>
+      </c>
+      <c r="B86" t="str">
+        <v>22009981</v>
+      </c>
+      <c r="C86" t="str">
+        <v>3223232339</v>
+      </c>
+      <c r="D86" t="str">
+        <v>jbauti1123124lavijo@gmail.com</v>
+      </c>
+      <c r="E86" t="str">
+        <v>18</v>
+      </c>
+      <c r="F86" t="str">
+        <v>2312319</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>C2OCA-COL</v>
+      </c>
+      <c r="B87" t="str">
+        <v>220091</v>
+      </c>
+      <c r="C87" t="str">
+        <v>32232362</v>
+      </c>
+      <c r="D87" t="str">
+        <v>jbautivv3ijo@gmail.com</v>
+      </c>
+      <c r="E87" t="str">
+        <v>16</v>
+      </c>
+      <c r="F87" t="str">
+        <v>23123124</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B88" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C88" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D88" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E88" t="str">
+        <v>17</v>
+      </c>
+      <c r="F88" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B89" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C89" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D89" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E89" t="str">
+        <v>18</v>
+      </c>
+      <c r="F89" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B90" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C90" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D90" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E90" t="str">
+        <v>3</v>
+      </c>
+      <c r="F90" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B91" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C91" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D91" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E91" t="str">
+        <v>4</v>
+      </c>
+      <c r="F91" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B92" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C92" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D92" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E92" t="str">
+        <v>16</v>
+      </c>
+      <c r="F92" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B93" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C93" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D93" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E93" t="str">
+        <v>18</v>
+      </c>
+      <c r="F93" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B94" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C94" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D94" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E94" t="str">
+        <v>17</v>
+      </c>
+      <c r="F94" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B95" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C95" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D95" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E95" t="str">
+        <v>17</v>
+      </c>
+      <c r="F95" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B96" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C96" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D96" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E96" t="str">
+        <v>18</v>
+      </c>
+      <c r="F96" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B97" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C97" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D97" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E97" t="str">
+        <v>17</v>
+      </c>
+      <c r="F97" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B98" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C98" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D98" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E98" t="str">
+        <v>17</v>
+      </c>
+      <c r="F98" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B99" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C99" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D99" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E99" t="str">
+        <v>17</v>
+      </c>
+      <c r="F99" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B100" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C100" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D100" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E100" t="str">
+        <v>17</v>
+      </c>
+      <c r="F100" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B101" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C101" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D101" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E101" t="str">
+        <v>18</v>
+      </c>
+      <c r="F101" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B102" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C102" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D102" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E102" t="str">
+        <v>18</v>
+      </c>
+      <c r="F102" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B103" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C103" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D103" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E103" t="str">
+        <v>17</v>
+      </c>
+      <c r="F103" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B104" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C104" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D104" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E104" t="str">
+        <v>17</v>
+      </c>
+      <c r="F104" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B105" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C105" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D105" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E105" t="str">
+        <v>17</v>
+      </c>
+      <c r="F105" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B106" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C106" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D106" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E106" t="str">
+        <v>17</v>
+      </c>
+      <c r="F106" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B107" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C107" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D107" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E107" t="str">
+        <v>18</v>
+      </c>
+      <c r="F107" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B108" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C108" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D108" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E108" t="str">
+        <v>17</v>
+      </c>
+      <c r="F108" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B109" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C109" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D109" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E109" t="str">
+        <v>10</v>
+      </c>
+      <c r="F109" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B110" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C110" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D110" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E110" t="str">
+        <v>18</v>
+      </c>
+      <c r="F110" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B111" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C111" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D111" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E111" t="str">
+        <v>17</v>
+      </c>
+      <c r="F111" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B112" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C112" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D112" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E112" t="str">
+        <v>16</v>
+      </c>
+      <c r="F112" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B113" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C113" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D113" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E113" t="str">
+        <v>18</v>
+      </c>
+      <c r="F113" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B114" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C114" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D114" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E114" t="str">
+        <v>18</v>
+      </c>
+      <c r="F114" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B115" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C115" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D115" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E115" t="str">
+        <v>16</v>
+      </c>
+      <c r="F115" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B116" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C116" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D116" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E116" t="str">
+        <v>18</v>
+      </c>
+      <c r="F116" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>COCA-COLA</v>
+      </c>
+      <c r="B117" t="str">
+        <v>22009988</v>
+      </c>
+      <c r="C117" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D117" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E117" t="str">
+        <v>16</v>
+      </c>
+      <c r="F117" t="str">
+        <v>2312312</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>Nombre de la Empresa</v>
+      </c>
+      <c r="B118" t="str">
+        <v>33456789</v>
+      </c>
+      <c r="D118" t="str">
+        <v>empresa@example.com</v>
+      </c>
+      <c r="E118" t="str">
+        <v>1</v>
+      </c>
+      <c r="F118" t="str">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>COCA-CO12</v>
+      </c>
+      <c r="B119" t="str">
+        <v>2200998</v>
+      </c>
+      <c r="C119" t="str">
+        <v>3223236331</v>
+      </c>
+      <c r="D119" t="str">
+        <v>jpbautistac@udistrital.edu.co</v>
+      </c>
+      <c r="E119" t="str">
+        <v>19</v>
+      </c>
+      <c r="F119" t="str">
+        <v>312311</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>COCA</v>
+      </c>
+      <c r="B120" t="str">
+        <v>22009</v>
+      </c>
+      <c r="C120" t="str">
+        <v>32232363</v>
+      </c>
+      <c r="D120" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E120" t="str">
+        <v>17</v>
+      </c>
+      <c r="F120" t="str">
+        <v>31231108</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B121" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C121" t="str">
+        <v>4123212</v>
+      </c>
+      <c r="D121" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E121" t="str">
+        <v>17</v>
+      </c>
+      <c r="F121" t="str">
+        <v>100192812</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B122" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C122" t="str">
+        <v>3213122</v>
+      </c>
+      <c r="D122" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E122" t="str">
+        <v>17</v>
+      </c>
+      <c r="F122" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B123" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C123" t="str">
+        <v>3213122</v>
+      </c>
+      <c r="D123" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E123" t="str">
+        <v>19</v>
+      </c>
+      <c r="F123" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>Nom de la Empresa</v>
+      </c>
+      <c r="B124" t="str">
+        <v>3341789</v>
+      </c>
+      <c r="D124" t="str">
+        <v>empresa@examp12.com</v>
+      </c>
+      <c r="E124" t="str">
+        <v>3</v>
+      </c>
+      <c r="F124" t="str">
+        <v>10045678</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B125" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C125" t="str">
+        <v>3213122</v>
+      </c>
+      <c r="D125" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E125" t="str">
+        <v>14</v>
+      </c>
+      <c r="F125" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B126" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C126" t="str">
+        <v>3213122</v>
+      </c>
+      <c r="D126" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E126" t="str">
+        <v>17</v>
+      </c>
+      <c r="F126" t="str">
+        <v>32312777</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B127" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C127" t="str">
+        <v>3213122</v>
+      </c>
+      <c r="D127" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E127" t="str">
+        <v>18</v>
+      </c>
+      <c r="F127" t="str">
+        <v>4122222</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B128" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C128" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D128" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E128" t="str">
+        <v>18</v>
+      </c>
+      <c r="F128" t="str">
+        <v>32312777</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B129" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C129" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D129" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E129" t="str">
+        <v>16</v>
+      </c>
+      <c r="F129" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B130" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C130" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D130" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E130" t="str">
+        <v>18</v>
+      </c>
+      <c r="F130" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B131" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C131" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D131" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E131" t="str">
+        <v>17</v>
+      </c>
+      <c r="F131" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B132" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C132" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D132" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E132" t="str">
+        <v>19</v>
+      </c>
+      <c r="F132" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B133" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C133" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D133" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E133" t="str">
+        <v>18</v>
+      </c>
+      <c r="F133" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B134" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C134" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D134" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E134" t="str">
+        <v>16</v>
+      </c>
+      <c r="F134" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B135" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C135" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D135" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E135" t="str">
+        <v>15</v>
+      </c>
+      <c r="F135" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B136" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C136" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D136" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E136" t="str">
+        <v>17</v>
+      </c>
+      <c r="F136" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B137" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C137" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D137" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E137" t="str">
+        <v>18</v>
+      </c>
+      <c r="F137" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B138" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C138" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D138" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E138" t="str">
+        <v>17</v>
+      </c>
+      <c r="F138" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B139" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C139" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D139" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E139" t="str">
+        <v>10</v>
+      </c>
+      <c r="F139" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B140" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C140" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D140" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E140" t="str">
+        <v>16</v>
+      </c>
+      <c r="F140" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B141" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C141" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D141" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E141" t="str">
+        <v>12</v>
+      </c>
+      <c r="F141" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B142" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C142" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D142" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E142" t="str">
+        <v>14</v>
+      </c>
+      <c r="F142" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B143" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C143" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D143" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E143" t="str">
+        <v>13</v>
+      </c>
+      <c r="F143" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>masTurbin</v>
+      </c>
+      <c r="B144" t="str">
+        <v>3124123</v>
+      </c>
+      <c r="C144" t="str">
+        <v>31231288</v>
+      </c>
+      <c r="D144" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E144" t="str">
+        <v>17</v>
+      </c>
+      <c r="F144" t="str">
+        <v>32143123</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>COCA</v>
+      </c>
+      <c r="B145" t="str">
+        <v>22009</v>
+      </c>
+      <c r="C145" t="str">
+        <v>32232363</v>
+      </c>
+      <c r="D145" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E145" t="str">
+        <v>15</v>
+      </c>
+      <c r="F145" t="str">
+        <v>31231108</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>COCA</v>
+      </c>
+      <c r="B146" t="str">
+        <v>22009</v>
+      </c>
+      <c r="C146" t="str">
+        <v>32232363</v>
+      </c>
+      <c r="D146" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E146" t="str">
+        <v>14</v>
+      </c>
+      <c r="F146" t="str">
+        <v>31231108</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>COCA</v>
+      </c>
+      <c r="B147" t="str">
+        <v>22009</v>
+      </c>
+      <c r="C147" t="str">
+        <v>32232363</v>
+      </c>
+      <c r="D147" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E147" t="str">
+        <v>16</v>
+      </c>
+      <c r="F147" t="str">
+        <v>31231108</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F83"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F147"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Registro de personas naturales implementado
</commit_message>
<xml_diff>
--- a/registro_empresas.xlsx
+++ b/registro_empresas.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2893,16 +2893,33 @@
         <v>32232363</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>31231108</v>
+      </c>
+      <c r="B148" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="C148" t="str">
+        <v>Pablo Bautista</v>
+      </c>
+      <c r="D148" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E148" t="str">
+        <v>3223236339</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E147"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E148"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -5838,9 +5855,29 @@
         <v>31231108</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>COCA</v>
+      </c>
+      <c r="B148" t="str">
+        <v>22009</v>
+      </c>
+      <c r="C148" t="str">
+        <v>3223236339</v>
+      </c>
+      <c r="D148" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="E148" t="str">
+        <v>12</v>
+      </c>
+      <c r="F148" t="str">
+        <v>31231108</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F147"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F148"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>